<commit_message>
build : added some changes
</commit_message>
<xml_diff>
--- a/public/usersInfo.xlsx
+++ b/public/usersInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Videos-Meets-MrValizade\adminPanel-task\admin-panel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7892398D-9FBF-4D07-B2EE-D29601DA76E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDCFB65-F05B-4913-AE79-C3B67E47629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>firstName</t>
   </si>
@@ -48,9 +48,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>soheil</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>soheil@gmail.com</t>
   </si>
   <si>
-    <t>38e00db922f4845465040c2</t>
-  </si>
-  <si>
     <t>amin</t>
   </si>
   <si>
@@ -72,20 +66,29 @@
     <t>amin@gmail.com</t>
   </si>
   <si>
-    <t>58f00db922f4845465040c2</t>
-  </si>
-  <si>
     <t>05/12/2004'</t>
   </si>
   <si>
-    <t>09/0/2018'</t>
+    <t>sarvar</t>
+  </si>
+  <si>
+    <t>hojat</t>
+  </si>
+  <si>
+    <t>09/06/2018'</t>
+  </si>
+  <si>
+    <t>hojat@gmail.com</t>
+  </si>
+  <si>
+    <t>02/07/2015'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,12 +109,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,10 +138,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -426,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,10 +435,9 @@
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,22 +459,19 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>123456789</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E2">
         <v>9357984285</v>
@@ -489,24 +480,21 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
       <c r="C3">
         <v>987654321</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E3">
         <v>963258741</v>
@@ -515,18 +503,39 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
+      <c r="C4">
+        <v>1203659875</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>6543653</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{6AAF9155-87EF-4716-99E2-27C504E19DEA}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{D6D6D793-9687-4E23-8678-F399EB575637}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{BD019225-3863-4FB2-B95C-2FC9BFF8A283}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>